<commit_message>
Added TestData sheet and a few test cases
</commit_message>
<xml_diff>
--- a/TestCase Repository.xlsx
+++ b/TestCase Repository.xlsx
@@ -13,13 +13,14 @@
   </bookViews>
   <sheets>
     <sheet name="TestSuite1" sheetId="1" r:id="rId1"/>
+    <sheet name="TestData" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="44">
   <si>
     <t>Test Case</t>
   </si>
@@ -120,6 +121,62 @@
   </si>
   <si>
     <t>/wallet/v1/customers/create</t>
+  </si>
+  <si>
+    <t>WalletRegistration</t>
+  </si>
+  <si>
+    <t>P_WalletRegister</t>
+  </si>
+  <si>
+    <t>Create new customer- All valid details</t>
+  </si>
+  <si>
+    <t>{
+"status": "success",
+"status_msg": "Customer created successfully",
+"consumer_id": $$new_cust_id
+}</t>
+  </si>
+  <si>
+    <t>TC04</t>
+  </si>
+  <si>
+    <t>new_cust_id</t>
+  </si>
+  <si>
+    <t>old_mobNo</t>
+  </si>
+  <si>
+    <t>old_cust_id</t>
+  </si>
+  <si>
+    <t>old_email_id</t>
+  </si>
+  <si>
+    <t>cust_id_zero_bal</t>
+  </si>
+  <si>
+    <t>abc@bc.com</t>
+  </si>
+  <si>
+    <t>test@gmail.com</t>
+  </si>
+  <si>
+    <t>#new_mobNo</t>
+  </si>
+  <si>
+    <t>#new_email_id</t>
+  </si>
+  <si>
+    <t>TC05</t>
+  </si>
+  <si>
+    <t>{ 
+"mobileNo":#new_mobNo, 
+"email":#new_email_id,
+"name_of_customer":"TestUser"
+}</t>
   </si>
 </sst>
 </file>
@@ -179,7 +236,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -189,6 +246,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -504,10 +564,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AD4"/>
+  <dimension ref="A1:AD7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -686,8 +746,205 @@
       <c r="Z4" s="1"/>
       <c r="AA4" s="1"/>
     </row>
+    <row r="5" spans="1:30" ht="84.75" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="I5" s="4">
+        <v>201</v>
+      </c>
+      <c r="J5" s="1"/>
+      <c r="K5" s="1"/>
+      <c r="L5" s="1"/>
+      <c r="M5" s="1"/>
+      <c r="N5" s="1"/>
+      <c r="O5" s="1"/>
+      <c r="P5" s="1"/>
+      <c r="Q5" s="1"/>
+      <c r="R5" s="1"/>
+      <c r="S5" s="1"/>
+      <c r="T5" s="1"/>
+      <c r="U5" s="1"/>
+      <c r="V5" s="1"/>
+      <c r="W5" s="1"/>
+      <c r="X5" s="1"/>
+      <c r="Y5" s="1"/>
+      <c r="Z5" s="1"/>
+      <c r="AA5" s="1"/>
+      <c r="AB5" s="1"/>
+      <c r="AC5" s="1"/>
+      <c r="AD5" s="1"/>
+    </row>
+    <row r="6" spans="1:30" ht="84.75" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="I6" s="4">
+        <v>201</v>
+      </c>
+      <c r="J6" s="1"/>
+      <c r="K6" s="1"/>
+      <c r="L6" s="1"/>
+      <c r="M6" s="1"/>
+      <c r="N6" s="1"/>
+      <c r="O6" s="1"/>
+      <c r="P6" s="1"/>
+      <c r="Q6" s="1"/>
+      <c r="R6" s="1"/>
+      <c r="S6" s="1"/>
+      <c r="T6" s="1"/>
+      <c r="U6" s="1"/>
+      <c r="V6" s="1"/>
+      <c r="W6" s="1"/>
+      <c r="X6" s="1"/>
+      <c r="Y6" s="1"/>
+      <c r="Z6" s="1"/>
+      <c r="AA6" s="1"/>
+      <c r="AB6" s="1"/>
+      <c r="AC6" s="1"/>
+      <c r="AD6" s="1"/>
+    </row>
+    <row r="7" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="G7" s="1"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.42578125" customWidth="1"/>
+    <col min="2" max="2" width="13.7109375" customWidth="1"/>
+    <col min="3" max="3" width="16.42578125" customWidth="1"/>
+    <col min="4" max="4" width="16.140625" customWidth="1"/>
+    <col min="5" max="5" width="18.7109375" customWidth="1"/>
+    <col min="6" max="6" width="15.140625" customWidth="1"/>
+    <col min="7" max="7" width="17.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="24.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="4">
+        <v>9810101010</v>
+      </c>
+      <c r="B2" s="1"/>
+      <c r="C2" s="4">
+        <v>9833868977</v>
+      </c>
+      <c r="D2" s="4">
+        <v>833012</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="G2" s="4">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="4">
+        <v>9812231223</v>
+      </c>
+      <c r="B3" s="1"/>
+      <c r="C3" s="4">
+        <v>7720077155</v>
+      </c>
+      <c r="D3" s="4">
+        <v>143245</v>
+      </c>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="4">
+        <v>34567</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="1"/>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="4">
+        <v>1234567</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Get Method changes + test case additon + random generator
</commit_message>
<xml_diff>
--- a/TestCase Repository.xlsx
+++ b/TestCase Repository.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530"/>
   </bookViews>
   <sheets>
     <sheet name="TestSuite1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="182">
   <si>
     <t>Test Case</t>
   </si>
@@ -47,9 +47,6 @@
   </si>
   <si>
     <t>Expected status code</t>
-  </si>
-  <si>
-    <t>Parameters to validate</t>
   </si>
   <si>
     <t>Actual Result</t>
@@ -113,13 +110,6 @@
 }</t>
   </si>
   <si>
-    <t>{ 
-"mobileNo":"9833868977", 
-"email":"qc9167916845@gmail.com",
-"name_of_customer":"WLWTestTwo"
-}</t>
-  </si>
-  <si>
     <t>/wallet/v1/customers/create</t>
   </si>
   <si>
@@ -133,21 +123,6 @@
   </si>
   <si>
     <t>TC04</t>
-  </si>
-  <si>
-    <t>new_cust_id</t>
-  </si>
-  <si>
-    <t>old_mobNo</t>
-  </si>
-  <si>
-    <t>old_cust_id</t>
-  </si>
-  <si>
-    <t>old_email_id</t>
-  </si>
-  <si>
-    <t>cust_id_zero_bal</t>
   </si>
   <si>
     <t>abc@bc.com</t>
@@ -174,13 +149,644 @@
 "status_msg": "Customer created successfully",
 "consumer_id": 123
 }</t>
+  </si>
+  <si>
+    <t>ActivationCheck</t>
+  </si>
+  <si>
+    <t>P_ActivationCheck</t>
+  </si>
+  <si>
+    <t>GET</t>
+  </si>
+  <si>
+    <t>{ "status": "success", 
+"message": "Customer is active", 
+"activation_code": "A" }</t>
+  </si>
+  <si>
+    <t>TC05</t>
+  </si>
+  <si>
+    <t>Correct consumer id</t>
+  </si>
+  <si>
+    <t>/wallet/v1/customers/activation_status</t>
+  </si>
+  <si>
+    <t>consumer_id/6723</t>
+  </si>
+  <si>
+    <t>TC06</t>
+  </si>
+  <si>
+    <t>N_ActivationCheck</t>
+  </si>
+  <si>
+    <t>Use a consumer id which is not existing in database</t>
+  </si>
+  <si>
+    <t>consumer_id/833012</t>
+  </si>
+  <si>
+    <t>{
+ "status": "error",
+ "status_msg": "Customer does not exists",
+ "error_code": 104
+ }</t>
+  </si>
+  <si>
+    <t>TC07</t>
+  </si>
+  <si>
+    <t>Check for a customer who has been registered but not activated</t>
+  </si>
+  <si>
+    <t>consumer_id/6724</t>
+  </si>
+  <si>
+    <t>{
+"status": "error",
+"status_msg": "Customer not activated",
+"error_code": 106
+}</t>
+  </si>
+  <si>
+    <t>TC08</t>
+  </si>
+  <si>
+    <t>Valid Mobile number</t>
+  </si>
+  <si>
+    <t>TC09</t>
+  </si>
+  <si>
+    <t>Pick a mobile number which is not registered yet</t>
+  </si>
+  <si>
+    <t>TC10</t>
+  </si>
+  <si>
+    <t>Invalid mobile number</t>
+  </si>
+  <si>
+    <t>Invalid Params</t>
+  </si>
+  <si>
+    <t>TC11</t>
+  </si>
+  <si>
+    <t>consumer_id/1434872</t>
+  </si>
+  <si>
+    <t>{
+  "status": "success",
+  "transactions": [
+    {
+      "type": "Reversed",
+      "amount": "2",
+      "refID": "1a232323a12abc340",
+      "creationTime": "2016-05-16 17:37:27"
+    },
+    {
+      "type": "Reversed",
+      "amount": "5",
+      "refID": "1a23232323a12abc340",
+      "creationTime": "2016-05-16 17:36:09"
+    },
+    {
+      "type": "Paid",
+      "amount": "10",
+      "refID": "REC100000000002635626",
+      "creationTime": "2016-05-16 17:34:48"
+    },
+    {
+      "type": "Paid",
+      "amount": "2",
+      "refID": "1a232323a12abc340",
+      "creationTime": "2016-05-16 17:30:41"
+    },
+    {
+      "type": "Voucher Loaded",
+      "amount": "20.00",
+      "refID": "V986860228249",
+      "creationTime": "2016-05-16 17:30:22"
+    }
+  ]
+}</t>
+  </si>
+  <si>
+    <t>Get Transaction</t>
+  </si>
+  <si>
+    <t>P_GetTransaction</t>
+  </si>
+  <si>
+    <t>Blabla</t>
+  </si>
+  <si>
+    <t>Voucher Load</t>
+  </si>
+  <si>
+    <t>P_VoucherLoad</t>
+  </si>
+  <si>
+    <t>/wallet/v1/vouchers/create</t>
+  </si>
+  <si>
+    <t>/wallet/v1/transactions/list</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+{ 
+"status": "success", 
+"message": "Voucher created Successfully", 
+"voucher_refID": "VRef1447848960410933" 
+}</t>
+  </si>
+  <si>
+    <t>{
+"status": "success",
+"vouchers": [
+{
+"voucher_type": "G",
+"amount": "30.00",
+"voucherID": "TEST1234TT",
+"creationTime": "2015-02-26 17:04:10",
+"expiryTime": "2015-12-26 17:04:10",
+"narration": "PizzaHut"
+}]
+}</t>
+  </si>
+  <si>
+    <t>/wallet/v1/vouchers/list</t>
+  </si>
+  <si>
+    <t>P_Get VoucherList</t>
+  </si>
+  <si>
+    <t>Credit Money - General Wallet</t>
+  </si>
+  <si>
+    <t>Valid and successful credit</t>
+  </si>
+  <si>
+    <t>{
+"status": "success",
+"message": "Customer wallet credited successfully",
+"amount": "10",
+"txnNo": 924259830594,
+"request_id": "4324342342",
+"transaction_time": "2015-02-18 18:45:15"
+}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/wallet/v1/credits/general </t>
+  </si>
+  <si>
+    <t>Credit Money General Wallet</t>
+  </si>
+  <si>
+    <t>General Wallet Balance Enquiry</t>
+  </si>
+  <si>
+    <t>Valid and successful get call</t>
+  </si>
+  <si>
+    <t>/wallet/v1/balances/general</t>
+  </si>
+  <si>
+    <t>/wallet/v1/balances/voucher</t>
+  </si>
+  <si>
+    <t>{
+ "status": "success",
+ "type": "Voucher",
+ "Balance": "10" 
+ }</t>
+  </si>
+  <si>
+    <t>Voucher Balance Enquiry</t>
+  </si>
+  <si>
+    <t>/wallet/v1/debits/general</t>
+  </si>
+  <si>
+    <t>Wallet Debit API</t>
+  </si>
+  <si>
+    <t>{
+  "status": "Success",
+  "message": "Customer wallet debited successfully",
+  "amount": "5",
+  "shmart_refID": "555405379028",
+  "transaction_time": "2016-06-03 15:40:41"
+}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{  
+    "consumer_id":"1434889",
+    "mobileNo" : "9823232323",
+    "total_amount" :"5", 
+    "email":"test@test.com", 
+    "merchant_refID":"1aaaaa340" 
+} </t>
+  </si>
+  <si>
+    <t>Wallet Direct Debit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/wallet/v1/debits/reverse </t>
+  </si>
+  <si>
+    <t>{
+"consumer_id" : "6103",
+"shmart_refID":"271720987929aaa"
+}</t>
+  </si>
+  <si>
+    <t>{
+"status": "error",
+"message": "No records found for shmart refID"
+}</t>
+  </si>
+  <si>
+    <t>Debit Reversal</t>
+  </si>
+  <si>
+    <t>Transaction Requery</t>
+  </si>
+  <si>
+    <t>merchant_refID/abc121212</t>
+  </si>
+  <si>
+    <t>/wallet/v1/requery/status</t>
+  </si>
+  <si>
+    <t>Add Beneficiary</t>
+  </si>
+  <si>
+    <t>Invalid Ref ID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{ 
+"beneficiary_accountNo" : "93333211034299", 
+"beneficiary_accountType" : "savings", 
+"beneficiary_name":"Test Ben1", 
+"beneficiary_mobileNo":"999999999",
+"consumer_id":"1434889",
+"ifsc_code":"HDFC0000088",
+"addr":"Hi tech plaza Mahacali caves road", 
+"mobileNo":"9167916845"
+} </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Valid Details 
+</t>
+  </si>
+  <si>
+    <t>/wallet/v1/transfers/create</t>
+  </si>
+  <si>
+    <t>TC12</t>
+  </si>
+  <si>
+    <t>TC13</t>
+  </si>
+  <si>
+    <t>TC14</t>
+  </si>
+  <si>
+    <t>TC15</t>
+  </si>
+  <si>
+    <t>TC16</t>
+  </si>
+  <si>
+    <t>TC17</t>
+  </si>
+  <si>
+    <t>TC18</t>
+  </si>
+  <si>
+    <t>TC19</t>
+  </si>
+  <si>
+    <t>TC20</t>
+  </si>
+  <si>
+    <t>TC21</t>
+  </si>
+  <si>
+    <t>{
+"status": "success",
+"consumer_id": "6723"
+}</t>
+  </si>
+  <si>
+    <t>{
+"status": "error",
+"message": "Customer does not exist",
+"error_code": "104"
+}</t>
+  </si>
+  <si>
+    <t>{ "status": "error", "message": "Parameter missing" }</t>
+  </si>
+  <si>
+    <t>Get Customer ID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/wallet/v1/customers/getConsumerID </t>
+  </si>
+  <si>
+    <t>{
+  "mobile_no":"9811223344"
+  }</t>
+  </si>
+  <si>
+    <t>{
+  "mobile_no":"9167185871"
+  }</t>
+  </si>
+  <si>
+    <t>{
+  "mobile_no":"abcd"
+  }</t>
+  </si>
+  <si>
+    <t>{
+"status": "success",
+"type": "General",
+"blocked_amount": 0,
+"balance": "10" 
+}</t>
+  </si>
+  <si>
+    <t>{
+"status": "error",
+"status_msg": "Transaction not found",
+"error_code": 361
+}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+{
+"status": "success",
+"status_msg": "Added beneficiary successfully",
+"BeneficiaryCode": "18767654"
+}
+</t>
+  </si>
+  <si>
+    <t>Valid_Details_GenerateOTP</t>
+  </si>
+  <si>
+    <t>Valid Ddetails</t>
+  </si>
+  <si>
+    <t>{
+"consumer_id":#old_cust_id
+}</t>
+  </si>
+  <si>
+    <t>{
+ "status": "success",
+ "message": "OTP Sent to customer mobile number"
+ }</t>
+  </si>
+  <si>
+    <t>Create new customer - Already used email id</t>
+  </si>
+  <si>
+    <t>{ 
+"mobileNo"9123451212", 
+"email":#old_email_id
+"name_of_customer":"WLWTestTwo"
+}</t>
+  </si>
+  <si>
+    <t>Create new customer - Already used mobile number</t>
+  </si>
+  <si>
+    <t>#new_cust_id</t>
+  </si>
+  <si>
+    <t>#old_mobNo</t>
+  </si>
+  <si>
+    <t>#old_cust_id</t>
+  </si>
+  <si>
+    <t>#old_email_id</t>
+  </si>
+  <si>
+    <t>#cust_id_zero_bal</t>
+  </si>
+  <si>
+    <t>{
+  "status": "error",
+  "message": " User with mobileNo already exists",
+  "error_code": "101"
+ }</t>
+  </si>
+  <si>
+    <t>{ 
+"mobileNo":#old_mobNo, 
+"email":#new_email_id,
+"name_of_customer":"TestUser"
+}</t>
+  </si>
+  <si>
+    <t>Create new customer - Pass a blank name or name with special characters</t>
+  </si>
+  <si>
+    <t>{ 
+"mobileNo":#new_mobNo, 
+"email":#new_email_id,
+"name_of_customer":" "
+}</t>
+  </si>
+  <si>
+    <t>{ "status": "error", "message": "Invalid parameter Name", "error_code": "157" }</t>
+  </si>
+  <si>
+    <t>Create new customer - Invalid mobile number. Only 10 digit mobile number can be used</t>
+  </si>
+  <si>
+    <t>{ 
+ "mobileNo":"9811", 
+ "email":"qcabcd@gmail.com",
+ "name_of_customer":" Test "
+ }</t>
+  </si>
+  <si>
+    <t>{
+  "status": "error",
+  "message": "Invalid mobile number. Only 10 digit mobile number can be used",
+  "error_code": "114
+ }</t>
+  </si>
+  <si>
+    <t>For a user who has been registered by Wallet Registration API, OTP has been generated but Registration OTP verification API has not been run</t>
+  </si>
+  <si>
+    <t>consumer_id/6725</t>
+  </si>
+  <si>
+    <t>{
+ "status": "error",
+ "status_msg": "User not activated , OTP activation is pending",
+ "error_code": 100
+ }</t>
+  </si>
+  <si>
+    <t>{
+  "mobileno":"XXXXXX"
+  }</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Successfully create a voucher
+</t>
+  </si>
+  <si>
+    <t>{
+ "amount":"15", 
+ "consumer_id":"1434872", 
+ "expiry_date":"20160607160000",
+ "voucher_type":"G",
+ "voucher_refID":#random_string
+}</t>
+  </si>
+  <si>
+    <t>Expiry date less than today's date</t>
+  </si>
+  <si>
+    <t>{
+ "amount":"15", 
+ "consumer_id":"1434872", 
+ "expiry_date":"20150607160000",
+ "voucher_type":"G",
+ "voucher_refID":#random_string
+}</t>
+  </si>
+  <si>
+    <t>{
+  "status": "error",
+  "message": "Invalid parameter Filler1",
+  "error_code": "427"
+}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Valid consumer_id of an existing customer </t>
+  </si>
+  <si>
+    <t>N_Get VoucherList</t>
+  </si>
+  <si>
+    <t>invalid details</t>
+  </si>
+  <si>
+    <t>consumer_id/abc</t>
+  </si>
+  <si>
+    <t>{ "status": "failed", "message": "Consumer does not exists" }</t>
+  </si>
+  <si>
+    <t>VoucherList</t>
+  </si>
+  <si>
+    <t>not registered consumer</t>
+  </si>
+  <si>
+    <t>consumer_id/1234500</t>
+  </si>
+  <si>
+    <t>Get Voucher list when there are no vouchers for that customer</t>
+  </si>
+  <si>
+    <t>{ "status": "success", "vouchers": [] }</t>
+  </si>
+  <si>
+    <t>Parameters to ignore</t>
+  </si>
+  <si>
+    <t>{
+  "status": "error",
+  "message": "Duplicate Voucher RefID",
+  "error_code": "111"
+}</t>
+  </si>
+  <si>
+    <t>{
+ "amount":"15", 
+ "consumer_id":"1434872", 
+ "expiry_date":"20180607160000",
+ "voucher_type":"G",
+ "voucher_refID":"LSDCIYCJHXMU"
+}</t>
+  </si>
+  <si>
+    <t>{
+"amount":"10",
+"consumer_id":"1434872",
+"request_id":#random_string
+}</t>
+  </si>
+  <si>
+    <t>TC22</t>
+  </si>
+  <si>
+    <t>TC23</t>
+  </si>
+  <si>
+    <t>TC24</t>
+  </si>
+  <si>
+    <t>TC25</t>
+  </si>
+  <si>
+    <t>TC26</t>
+  </si>
+  <si>
+    <t>TC27</t>
+  </si>
+  <si>
+    <t>TC28</t>
+  </si>
+  <si>
+    <t>TC29</t>
+  </si>
+  <si>
+    <t>TC30</t>
+  </si>
+  <si>
+    <t>TC31</t>
+  </si>
+  <si>
+    <t>voucher_refID</t>
+  </si>
+  <si>
+    <t>creationTime,expiryTime</t>
+  </si>
+  <si>
+    <t>txnNo, request_id,transaction_time</t>
+  </si>
+  <si>
+    <t>shmart_refID, transaction_time</t>
+  </si>
+  <si>
+    <t>BeneficiaryCode</t>
+  </si>
+  <si>
+    <t>refID,creationTime</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -200,8 +806,22 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -220,6 +840,36 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -230,10 +880,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -247,8 +898,32 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -561,10 +1236,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AD6"/>
+  <dimension ref="A1:AD32"/>
   <sheetViews>
-    <sheetView topLeftCell="C2" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J32" sqref="J32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -572,14 +1248,17 @@
     <col min="2" max="2" width="17" customWidth="1"/>
     <col min="3" max="3" width="18.7109375" customWidth="1"/>
     <col min="4" max="4" width="17.28515625" customWidth="1"/>
-    <col min="5" max="5" width="14.28515625" customWidth="1"/>
-    <col min="6" max="6" width="19.42578125" customWidth="1"/>
-    <col min="7" max="7" width="32.140625" customWidth="1"/>
-    <col min="8" max="8" width="24" customWidth="1"/>
+    <col min="5" max="5" width="9.42578125" customWidth="1"/>
+    <col min="6" max="6" width="23.85546875" customWidth="1"/>
+    <col min="7" max="7" width="30.42578125" customWidth="1"/>
+    <col min="8" max="8" width="39" customWidth="1"/>
     <col min="9" max="9" width="20.42578125" customWidth="1"/>
+    <col min="10" max="10" width="19.85546875" customWidth="1"/>
+    <col min="11" max="11" width="17.42578125" customWidth="1"/>
+    <col min="12" max="12" width="22" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" s="2" customFormat="1" ht="36" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:30" s="2" customFormat="1" ht="24" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -608,68 +1287,68 @@
         <v>8</v>
       </c>
       <c r="J1" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="K1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="L1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="2" t="s">
+    </row>
+    <row r="2" spans="1:30" s="1" customFormat="1" ht="60" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2" s="9" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="2" spans="1:30" s="1" customFormat="1" ht="72" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B2" s="1" t="s">
+      <c r="C2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="F2" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="G2" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="H2" s="1" t="s">
         <v>17</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>18</v>
       </c>
       <c r="I2" s="1">
         <v>400</v>
       </c>
     </row>
-    <row r="3" spans="1:30" ht="72.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:30" ht="60.75" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>21</v>
-      </c>
       <c r="H3" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I3" s="1">
         <v>400</v>
@@ -696,34 +1375,32 @@
       <c r="AC3" s="1"/>
       <c r="AD3" s="1"/>
     </row>
-    <row r="4" spans="1:30" ht="84.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:30" ht="60.75" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B4" s="1" t="s">
         <v>22</v>
       </c>
+      <c r="B4" s="9" t="s">
+        <v>11</v>
+      </c>
       <c r="C4" s="1" t="s">
-        <v>24</v>
+        <v>123</v>
       </c>
       <c r="D4" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="E4" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="F4" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="F4" s="1" t="s">
-        <v>27</v>
-      </c>
       <c r="G4" s="1" t="s">
-        <v>26</v>
+        <v>125</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="I4" s="1">
-        <v>400</v>
-      </c>
+        <v>126</v>
+      </c>
+      <c r="I4" s="1"/>
       <c r="J4" s="1"/>
       <c r="K4" s="1"/>
       <c r="L4" s="1"/>
@@ -742,34 +1419,37 @@
       <c r="Y4" s="1"/>
       <c r="Z4" s="1"/>
       <c r="AA4" s="1"/>
+      <c r="AB4" s="1"/>
+      <c r="AC4" s="1"/>
+      <c r="AD4" s="1"/>
     </row>
     <row r="5" spans="1:30" ht="72.75" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
+      </c>
+      <c r="B5" s="12" t="s">
+        <v>21</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>15</v>
+        <v>127</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>14</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>41</v>
+        <v>128</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="I5" s="4">
-        <v>201</v>
+        <v>24</v>
+      </c>
+      <c r="I5" s="1">
+        <v>400</v>
       </c>
       <c r="J5" s="1"/>
       <c r="K5" s="1"/>
@@ -789,12 +1469,816 @@
       <c r="Y5" s="1"/>
       <c r="Z5" s="1"/>
       <c r="AA5" s="1"/>
-      <c r="AB5" s="1"/>
-      <c r="AC5" s="1"/>
-      <c r="AD5" s="1"/>
-    </row>
-    <row r="6" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="G6" s="1"/>
+    </row>
+    <row r="6" spans="1:30" ht="72.75" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B6" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="I6" s="4">
+        <v>201</v>
+      </c>
+      <c r="J6" s="1"/>
+      <c r="K6" s="1"/>
+      <c r="L6" s="1"/>
+      <c r="M6" s="1"/>
+      <c r="N6" s="1"/>
+      <c r="O6" s="1"/>
+      <c r="P6" s="1"/>
+      <c r="Q6" s="1"/>
+      <c r="R6" s="1"/>
+      <c r="S6" s="1"/>
+      <c r="T6" s="1"/>
+      <c r="U6" s="1"/>
+      <c r="V6" s="1"/>
+      <c r="W6" s="1"/>
+      <c r="X6" s="1"/>
+      <c r="Y6" s="1"/>
+      <c r="Z6" s="1"/>
+      <c r="AA6" s="1"/>
+      <c r="AB6" s="1"/>
+      <c r="AC6" s="1"/>
+      <c r="AD6" s="1"/>
+    </row>
+    <row r="7" spans="1:30" ht="72.75" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B7" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="I7" s="4"/>
+      <c r="J7" s="1"/>
+      <c r="K7" s="1"/>
+      <c r="L7" s="1"/>
+      <c r="M7" s="1"/>
+      <c r="N7" s="1"/>
+      <c r="O7" s="1"/>
+      <c r="P7" s="1"/>
+      <c r="Q7" s="1"/>
+      <c r="R7" s="1"/>
+      <c r="S7" s="1"/>
+      <c r="T7" s="1"/>
+      <c r="U7" s="1"/>
+      <c r="V7" s="1"/>
+      <c r="W7" s="1"/>
+      <c r="X7" s="1"/>
+      <c r="Y7" s="1"/>
+      <c r="Z7" s="1"/>
+      <c r="AA7" s="1"/>
+      <c r="AB7" s="1"/>
+      <c r="AC7" s="1"/>
+      <c r="AD7" s="1"/>
+    </row>
+    <row r="8" spans="1:30" ht="60.75" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B8" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="I8" s="4"/>
+      <c r="J8" s="1"/>
+      <c r="K8" s="1"/>
+      <c r="L8" s="1"/>
+      <c r="M8" s="1"/>
+      <c r="N8" s="1"/>
+      <c r="O8" s="1"/>
+      <c r="P8" s="1"/>
+      <c r="Q8" s="1"/>
+      <c r="R8" s="1"/>
+      <c r="S8" s="1"/>
+      <c r="T8" s="1"/>
+      <c r="U8" s="1"/>
+      <c r="V8" s="1"/>
+      <c r="W8" s="1"/>
+      <c r="X8" s="1"/>
+      <c r="Y8" s="1"/>
+      <c r="Z8" s="1"/>
+      <c r="AA8" s="1"/>
+      <c r="AB8" s="1"/>
+      <c r="AC8" s="1"/>
+      <c r="AD8" s="1"/>
+    </row>
+    <row r="9" spans="1:30" ht="72.75" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B9" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="I9" s="4"/>
+      <c r="J9" s="1"/>
+      <c r="K9" s="1"/>
+      <c r="L9" s="1"/>
+      <c r="M9" s="1"/>
+      <c r="N9" s="1"/>
+      <c r="O9" s="1"/>
+      <c r="P9" s="1"/>
+      <c r="Q9" s="1"/>
+      <c r="R9" s="1"/>
+      <c r="S9" s="1"/>
+      <c r="T9" s="1"/>
+      <c r="U9" s="1"/>
+      <c r="V9" s="1"/>
+      <c r="W9" s="1"/>
+      <c r="X9" s="1"/>
+      <c r="Y9" s="1"/>
+      <c r="Z9" s="1"/>
+      <c r="AA9" s="1"/>
+      <c r="AB9" s="1"/>
+      <c r="AC9" s="1"/>
+      <c r="AD9" s="1"/>
+    </row>
+    <row r="10" spans="1:30" ht="36.75" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B10" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="11" spans="1:30" ht="60.75" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B11" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="12" spans="1:30" ht="96.75" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B12" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="13" spans="1:30" ht="60.75" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="B13" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="14" spans="1:30" ht="48.75" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="B14" s="11" t="s">
+        <v>115</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="15" spans="1:30" ht="60.75" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="B15" s="11" t="s">
+        <v>115</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="16" spans="1:30" ht="60.75" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="B16" s="11" t="s">
+        <v>115</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="H16" s="1" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" ht="36.75" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B17" s="11" t="s">
+        <v>115</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" s="1" customFormat="1" ht="84" x14ac:dyDescent="0.2">
+      <c r="A18" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="B18" s="13" t="s">
+        <v>66</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="H18" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="J18" s="1" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" s="1" customFormat="1" ht="84" x14ac:dyDescent="0.2">
+      <c r="A19" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="B19" s="13" t="s">
+        <v>66</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="H19" s="1" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" s="1" customFormat="1" ht="84" x14ac:dyDescent="0.2">
+      <c r="A20" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="B20" s="13" t="s">
+        <v>66</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="H20" s="1" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" ht="144.75" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="B21" s="12" t="s">
+        <v>157</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="F21" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="H21" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="J21" s="1" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" ht="24.75" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="B22" s="12" t="s">
+        <v>157</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="F22" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="H22" s="1" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" ht="24.75" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="B23" s="12" t="s">
+        <v>157</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="F23" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="H23" s="1" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" ht="48.75" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="B24" s="12" t="s">
+        <v>157</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="F24" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="G24" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="H24" s="7" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" ht="108.75" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="B25" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="G25" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="H25" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="J25" s="1" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" ht="72.75" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="B26" s="12" t="s">
+        <v>79</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="G26" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="H26" s="1" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" ht="75" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="B27" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="G27" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="H27" s="5" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" ht="135" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="B28" s="12" t="s">
+        <v>89</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F28" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="G28" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="H28" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="J28" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" ht="48.75" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="B29" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F29" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="G29" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="H29" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" ht="60.75" x14ac:dyDescent="0.25">
+      <c r="A30" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="B30" s="12" t="s">
+        <v>94</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="F30" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="G30" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="H30" s="1" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" s="1" customFormat="1" ht="168" x14ac:dyDescent="0.2">
+      <c r="A31" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="B31" s="8" t="s">
+        <v>97</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F31" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="G31" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="H31" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="J31" s="1" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" ht="409.6" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="B32" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="C32" t="s">
+        <v>64</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="E32" t="s">
+        <v>38</v>
+      </c>
+      <c r="F32" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="G32" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="H32" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="J32" s="1" t="s">
+        <v>181</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -806,8 +2290,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -823,28 +2307,28 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>32</v>
+        <v>130</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>40</v>
-      </c>
       <c r="F1" s="1" t="s">
-        <v>35</v>
+        <v>133</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="4">
         <v>9810121212</v>
       </c>
@@ -856,10 +2340,10 @@
         <v>833012</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>38</v>
+        <v>30</v>
+      </c>
+      <c r="F2" s="10" t="s">
+        <v>31</v>
       </c>
       <c r="G2" s="4">
         <v>123</v>
@@ -894,6 +2378,9 @@
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="F2" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Code changes to incorporate SOAP request handling
</commit_message>
<xml_diff>
--- a/TestCase Repository.xlsx
+++ b/TestCase Repository.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="785" uniqueCount="388">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="785" uniqueCount="391">
   <si>
     <t>Test Case</t>
   </si>
@@ -1801,6 +1801,15 @@
 "email":#old_email_id
 "name_of_customer":"WLWTestTwo"
 }</t>
+  </si>
+  <si>
+    <t>TC82</t>
+  </si>
+  <si>
+    <t>TC83</t>
+  </si>
+  <si>
+    <t>TC84</t>
   </si>
 </sst>
 </file>
@@ -2286,8 +2295,8 @@
   <dimension ref="A1:AD85"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G11" sqref="G11"/>
+      <pane ySplit="1" topLeftCell="A83" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B90" sqref="B90"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2529,7 +2538,7 @@
     </row>
     <row r="6" spans="1:30" ht="84.75" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>27</v>
+        <v>37</v>
       </c>
       <c r="B6" s="11" t="s">
         <v>20</v>
@@ -2578,7 +2587,7 @@
     </row>
     <row r="7" spans="1:30" ht="72.75" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="B7" s="11" t="s">
         <v>24</v>
@@ -2630,7 +2639,7 @@
     </row>
     <row r="8" spans="1:30" ht="72.75" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="B8" s="11" t="s">
         <v>24</v>
@@ -2680,7 +2689,7 @@
     </row>
     <row r="9" spans="1:30" ht="60.75" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="B9" s="11" t="s">
         <v>24</v>
@@ -2730,7 +2739,7 @@
     </row>
     <row r="10" spans="1:30" ht="72.75" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="B10" s="11" t="s">
         <v>24</v>
@@ -2780,7 +2789,7 @@
     </row>
     <row r="11" spans="1:30" ht="72.75" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="B11" s="11" t="s">
         <v>24</v>
@@ -2830,7 +2839,7 @@
     </row>
     <row r="12" spans="1:30" ht="60.75" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="B12" s="11" t="s">
         <v>24</v>
@@ -2880,7 +2889,7 @@
     </row>
     <row r="13" spans="1:30" ht="72.75" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>50</v>
+        <v>88</v>
       </c>
       <c r="B13" s="12" t="s">
         <v>34</v>
@@ -2909,7 +2918,7 @@
     </row>
     <row r="14" spans="1:30" ht="60.75" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>52</v>
+        <v>89</v>
       </c>
       <c r="B14" s="12" t="s">
         <v>34</v>
@@ -2938,7 +2947,7 @@
     </row>
     <row r="15" spans="1:30" ht="96.75" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>55</v>
+        <v>90</v>
       </c>
       <c r="B15" s="12" t="s">
         <v>42</v>
@@ -2967,7 +2976,7 @@
     </row>
     <row r="16" spans="1:30" ht="72.75" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="B16" s="12" t="s">
         <v>42</v>
@@ -2996,7 +3005,7 @@
     </row>
     <row r="17" spans="1:10" ht="84.75" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="B17" s="12" t="s">
         <v>42</v>
@@ -3025,7 +3034,7 @@
     </row>
     <row r="18" spans="1:10" ht="48.75" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="B18" s="10" t="s">
         <v>100</v>
@@ -3054,7 +3063,7 @@
     </row>
     <row r="19" spans="1:10" ht="60.75" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="B19" s="10" t="s">
         <v>100</v>
@@ -3083,7 +3092,7 @@
     </row>
     <row r="20" spans="1:10" ht="60.75" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="B20" s="10" t="s">
         <v>100</v>
@@ -3112,7 +3121,7 @@
     </row>
     <row r="21" spans="1:10" ht="36.75" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="B21" s="10" t="s">
         <v>100</v>
@@ -3141,7 +3150,7 @@
     </row>
     <row r="22" spans="1:10" s="1" customFormat="1" ht="84" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="B22" s="12" t="s">
         <v>59</v>
@@ -3170,7 +3179,7 @@
     </row>
     <row r="23" spans="1:10" s="1" customFormat="1" ht="84" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
-        <v>95</v>
+        <v>142</v>
       </c>
       <c r="B23" s="12" t="s">
         <v>59</v>
@@ -3199,7 +3208,7 @@
     </row>
     <row r="24" spans="1:10" s="1" customFormat="1" ht="84" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
-        <v>96</v>
+        <v>143</v>
       </c>
       <c r="B24" s="12" t="s">
         <v>59</v>
@@ -3228,7 +3237,7 @@
     </row>
     <row r="25" spans="1:10" ht="180.75" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>97</v>
+        <v>144</v>
       </c>
       <c r="B25" s="11" t="s">
         <v>134</v>
@@ -3257,7 +3266,7 @@
     </row>
     <row r="26" spans="1:10" ht="24.75" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
       <c r="B26" s="11" t="s">
         <v>134</v>
@@ -3286,7 +3295,7 @@
     </row>
     <row r="27" spans="1:10" ht="24.75" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>143</v>
+        <v>146</v>
       </c>
       <c r="B27" s="11" t="s">
         <v>134</v>
@@ -3315,7 +3324,7 @@
     </row>
     <row r="28" spans="1:10" ht="48.75" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>144</v>
+        <v>147</v>
       </c>
       <c r="B28" s="11" t="s">
         <v>134</v>
@@ -3344,7 +3353,7 @@
     </row>
     <row r="29" spans="1:10" ht="108.75" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
       <c r="B29" s="7" t="s">
         <v>65</v>
@@ -3373,7 +3382,7 @@
     </row>
     <row r="30" spans="1:10" ht="60.75" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="B30" s="7" t="s">
         <v>65</v>
@@ -3402,7 +3411,7 @@
     </row>
     <row r="31" spans="1:10" ht="72.75" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>147</v>
+        <v>150</v>
       </c>
       <c r="B31" s="7" t="s">
         <v>65</v>
@@ -3431,7 +3440,7 @@
     </row>
     <row r="32" spans="1:10" ht="72.75" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="B32" s="11" t="s">
         <v>70</v>
@@ -3460,7 +3469,7 @@
     </row>
     <row r="33" spans="1:10" ht="60.75" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>149</v>
+        <v>174</v>
       </c>
       <c r="B33" s="11" t="s">
         <v>70</v>
@@ -3489,7 +3498,7 @@
     </row>
     <row r="34" spans="1:10" ht="60.75" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>150</v>
+        <v>175</v>
       </c>
       <c r="B34" s="11" t="s">
         <v>70</v>
@@ -3518,7 +3527,7 @@
     </row>
     <row r="35" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>151</v>
+        <v>176</v>
       </c>
       <c r="B35" s="7" t="s">
         <v>74</v>
@@ -3547,7 +3556,7 @@
     </row>
     <row r="36" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>174</v>
+        <v>203</v>
       </c>
       <c r="B36" s="7" t="s">
         <v>74</v>
@@ -3576,7 +3585,7 @@
     </row>
     <row r="37" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="B37" s="7" t="s">
         <v>74</v>
@@ -3605,7 +3614,7 @@
     </row>
     <row r="38" spans="1:10" ht="135" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="B38" s="11" t="s">
         <v>77</v>
@@ -3634,7 +3643,7 @@
     </row>
     <row r="39" spans="1:10" ht="96.75" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
-        <v>203</v>
+        <v>179</v>
       </c>
       <c r="B39" s="11" t="s">
         <v>77</v>
@@ -3663,7 +3672,7 @@
     </row>
     <row r="40" spans="1:10" ht="72.75" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
-        <v>177</v>
+        <v>180</v>
       </c>
       <c r="B40" s="7" t="s">
         <v>80</v>
@@ -3692,7 +3701,7 @@
     </row>
     <row r="41" spans="1:10" ht="78.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
-        <v>178</v>
+        <v>204</v>
       </c>
       <c r="B41" s="11" t="s">
         <v>81</v>
@@ -3721,7 +3730,7 @@
     </row>
     <row r="42" spans="1:10" ht="84.75" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
-        <v>179</v>
+        <v>205</v>
       </c>
       <c r="B42" s="11" t="s">
         <v>81</v>
@@ -3750,7 +3759,7 @@
     </row>
     <row r="43" spans="1:10" ht="72.75" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
-        <v>180</v>
+        <v>206</v>
       </c>
       <c r="B43" s="11" t="s">
         <v>81</v>
@@ -3779,7 +3788,7 @@
     </row>
     <row r="44" spans="1:10" ht="72.75" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="B44" s="11" t="s">
         <v>81</v>
@@ -3808,7 +3817,7 @@
     </row>
     <row r="45" spans="1:10" ht="72.75" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
-        <v>205</v>
+        <v>208</v>
       </c>
       <c r="B45" s="11" t="s">
         <v>81</v>
@@ -3837,7 +3846,7 @@
     </row>
     <row r="46" spans="1:10" ht="72.75" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
-        <v>206</v>
+        <v>209</v>
       </c>
       <c r="B46" s="11" t="s">
         <v>81</v>
@@ -3866,7 +3875,7 @@
     </row>
     <row r="47" spans="1:10" s="1" customFormat="1" ht="120" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
-        <v>207</v>
+        <v>210</v>
       </c>
       <c r="B47" s="7" t="s">
         <v>84</v>
@@ -3895,7 +3904,7 @@
     </row>
     <row r="48" spans="1:10" s="1" customFormat="1" ht="120" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
-        <v>208</v>
+        <v>211</v>
       </c>
       <c r="B48" s="7" t="s">
         <v>84</v>
@@ -3924,7 +3933,7 @@
     </row>
     <row r="49" spans="1:10" s="1" customFormat="1" ht="120" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
       <c r="B49" s="7" t="s">
         <v>84</v>
@@ -3953,7 +3962,7 @@
     </row>
     <row r="50" spans="1:10" s="1" customFormat="1" ht="144.75" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
-        <v>210</v>
+        <v>213</v>
       </c>
       <c r="B50" s="7" t="s">
         <v>84</v>
@@ -3982,7 +3991,7 @@
     </row>
     <row r="51" spans="1:10" s="1" customFormat="1" ht="108.75" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
-        <v>211</v>
+        <v>214</v>
       </c>
       <c r="B51" s="7" t="s">
         <v>84</v>
@@ -4011,7 +4020,7 @@
     </row>
     <row r="52" spans="1:10" s="1" customFormat="1" ht="120" x14ac:dyDescent="0.2">
       <c r="A52" s="1" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="B52" s="7" t="s">
         <v>84</v>
@@ -4040,7 +4049,7 @@
     </row>
     <row r="53" spans="1:10" s="1" customFormat="1" ht="120" x14ac:dyDescent="0.2">
       <c r="A53" s="1" t="s">
-        <v>213</v>
+        <v>216</v>
       </c>
       <c r="B53" s="7" t="s">
         <v>84</v>
@@ -4069,7 +4078,7 @@
     </row>
     <row r="54" spans="1:10" s="1" customFormat="1" ht="120.75" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
-        <v>214</v>
+        <v>217</v>
       </c>
       <c r="B54" s="7" t="s">
         <v>84</v>
@@ -4098,7 +4107,7 @@
     </row>
     <row r="55" spans="1:10" s="1" customFormat="1" ht="120.75" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
-        <v>215</v>
+        <v>275</v>
       </c>
       <c r="B55" s="7" t="s">
         <v>84</v>
@@ -4127,7 +4136,7 @@
     </row>
     <row r="56" spans="1:10" ht="195" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
-        <v>216</v>
+        <v>276</v>
       </c>
       <c r="B56" s="15" t="s">
         <v>199</v>
@@ -4157,7 +4166,7 @@
     </row>
     <row r="57" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
-        <v>217</v>
+        <v>277</v>
       </c>
       <c r="B57" s="15" t="s">
         <v>199</v>
@@ -4186,7 +4195,7 @@
     </row>
     <row r="58" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
-        <v>275</v>
+        <v>278</v>
       </c>
       <c r="B58" s="15" t="s">
         <v>199</v>
@@ -4215,7 +4224,7 @@
     </row>
     <row r="59" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
-        <v>276</v>
+        <v>279</v>
       </c>
       <c r="B59" s="15" t="s">
         <v>199</v>
@@ -4244,7 +4253,7 @@
     </row>
     <row r="60" spans="1:10" ht="96.75" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
-        <v>277</v>
+        <v>280</v>
       </c>
       <c r="B60" s="16" t="s">
         <v>244</v>
@@ -4273,7 +4282,7 @@
     </row>
     <row r="61" spans="1:10" ht="72.75" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
-        <v>278</v>
+        <v>281</v>
       </c>
       <c r="B61" s="16" t="s">
         <v>244</v>
@@ -4302,7 +4311,7 @@
     </row>
     <row r="62" spans="1:10" ht="96.75" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
-        <v>279</v>
+        <v>282</v>
       </c>
       <c r="B62" s="16" t="s">
         <v>244</v>
@@ -4331,7 +4340,7 @@
     </row>
     <row r="63" spans="1:10" ht="72.75" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
-        <v>280</v>
+        <v>283</v>
       </c>
       <c r="B63" s="16" t="s">
         <v>244</v>
@@ -4360,7 +4369,7 @@
     </row>
     <row r="64" spans="1:10" ht="150" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
-        <v>281</v>
+        <v>346</v>
       </c>
       <c r="B64" s="16" t="s">
         <v>244</v>
@@ -4389,7 +4398,7 @@
     </row>
     <row r="65" spans="1:10" ht="90" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
-        <v>282</v>
+        <v>347</v>
       </c>
       <c r="B65" s="16" t="s">
         <v>244</v>
@@ -4418,7 +4427,7 @@
     </row>
     <row r="66" spans="1:10" ht="165" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
-        <v>283</v>
+        <v>348</v>
       </c>
       <c r="B66" s="16" t="s">
         <v>244</v>
@@ -4447,7 +4456,7 @@
     </row>
     <row r="67" spans="1:10" ht="150" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
-        <v>346</v>
+        <v>349</v>
       </c>
       <c r="B67" s="16" t="s">
         <v>244</v>
@@ -4476,7 +4485,7 @@
     </row>
     <row r="68" spans="1:10" ht="409.6" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
-        <v>347</v>
+        <v>350</v>
       </c>
       <c r="B68" s="11" t="s">
         <v>273</v>
@@ -4505,7 +4514,7 @@
     </row>
     <row r="69" spans="1:10" ht="60.75" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
-        <v>348</v>
+        <v>351</v>
       </c>
       <c r="B69" s="11" t="s">
         <v>273</v>
@@ -4534,7 +4543,7 @@
     </row>
     <row r="70" spans="1:10" ht="48.75" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
-        <v>349</v>
+        <v>352</v>
       </c>
       <c r="B70" s="11" t="s">
         <v>273</v>
@@ -4563,7 +4572,7 @@
     </row>
     <row r="71" spans="1:10" ht="90" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
-        <v>350</v>
+        <v>353</v>
       </c>
       <c r="B71" s="16" t="s">
         <v>296</v>
@@ -4592,7 +4601,7 @@
     </row>
     <row r="72" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
-        <v>351</v>
+        <v>354</v>
       </c>
       <c r="B72" s="16" t="s">
         <v>296</v>
@@ -4621,7 +4630,7 @@
     </row>
     <row r="73" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
-        <v>352</v>
+        <v>355</v>
       </c>
       <c r="B73" s="16" t="s">
         <v>296</v>
@@ -4650,7 +4659,7 @@
     </row>
     <row r="74" spans="1:10" ht="90" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
-        <v>353</v>
+        <v>356</v>
       </c>
       <c r="B74" s="16" t="s">
         <v>296</v>
@@ -4679,7 +4688,7 @@
     </row>
     <row r="75" spans="1:10" ht="135" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
-        <v>354</v>
+        <v>357</v>
       </c>
       <c r="B75" s="15" t="s">
         <v>317</v>
@@ -4708,7 +4717,7 @@
     </row>
     <row r="76" spans="1:10" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
-        <v>355</v>
+        <v>358</v>
       </c>
       <c r="B76" s="15" t="s">
         <v>317</v>
@@ -4737,7 +4746,7 @@
     </row>
     <row r="77" spans="1:10" ht="135" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
-        <v>356</v>
+        <v>359</v>
       </c>
       <c r="B77" s="15" t="s">
         <v>317</v>
@@ -4766,7 +4775,7 @@
     </row>
     <row r="78" spans="1:10" ht="135" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
-        <v>357</v>
+        <v>360</v>
       </c>
       <c r="B78" s="15" t="s">
         <v>317</v>
@@ -4795,7 +4804,7 @@
     </row>
     <row r="79" spans="1:10" ht="135" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
-        <v>358</v>
+        <v>361</v>
       </c>
       <c r="B79" s="15" t="s">
         <v>317</v>
@@ -4824,7 +4833,7 @@
     </row>
     <row r="80" spans="1:10" ht="135" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
-        <v>359</v>
+        <v>362</v>
       </c>
       <c r="B80" s="15" t="s">
         <v>317</v>
@@ -4853,7 +4862,7 @@
     </row>
     <row r="81" spans="1:10" ht="150" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
-        <v>360</v>
+        <v>372</v>
       </c>
       <c r="B81" s="19" t="s">
         <v>335</v>
@@ -4879,7 +4888,7 @@
     </row>
     <row r="82" spans="1:10" ht="150" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
-        <v>361</v>
+        <v>373</v>
       </c>
       <c r="B82" s="19" t="s">
         <v>335</v>
@@ -4905,12 +4914,12 @@
     </row>
     <row r="83" spans="1:10" ht="150" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
-        <v>362</v>
+        <v>388</v>
       </c>
       <c r="B83" s="19" t="s">
         <v>335</v>
       </c>
-      <c r="D83" s="17" t="s">
+      <c r="D83" s="1" t="s">
         <v>337</v>
       </c>
       <c r="E83" t="s">
@@ -4931,7 +4940,7 @@
     </row>
     <row r="84" spans="1:10" ht="72.75" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
-        <v>372</v>
+        <v>389</v>
       </c>
       <c r="B84" s="11" t="s">
         <v>65</v>
@@ -4960,7 +4969,7 @@
     </row>
     <row r="85" spans="1:10" ht="72.75" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
-        <v>373</v>
+        <v>390</v>
       </c>
       <c r="B85" s="11" t="s">
         <v>65</v>
@@ -4998,7 +5007,7 @@
   <dimension ref="A1:R14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10:A11"/>
+      <selection activeCell="J16" sqref="J16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>